<commit_message>
Todos los excel generados (Luis añadió más) y nuevo script de la base de datos
</commit_message>
<xml_diff>
--- a/API con Seguridad Implementada/Spring Initialzr/reto/equipos.xlsx
+++ b/API con Seguridad Implementada/Spring Initialzr/reto/equipos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="64">
   <si>
     <t>ID</t>
   </si>
@@ -56,7 +56,7 @@
     <t>JJJ</t>
   </si>
   <si>
-    <t>Hostia</t>
+    <t>aa</t>
   </si>
   <si>
     <t>Estación de trabajo potente para diseño gráfico</t>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>KAAAAA</t>
+  </si>
+  <si>
+    <t>gg</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
@@ -837,7 +843,7 @@
         <v>58</v>
       </c>
       <c r="F20" t="s" s="0">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="G20" t="s" s="0">
         <v>15</v>
@@ -866,7 +872,7 @@
         <v>58</v>
       </c>
       <c r="F21" t="s" s="0">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="G21" t="s" s="0">
         <v>15</v>
@@ -895,7 +901,7 @@
         <v>13</v>
       </c>
       <c r="F22" t="s" s="0">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="G22" t="s" s="0">
         <v>15</v>
@@ -924,7 +930,7 @@
         <v>13</v>
       </c>
       <c r="F23" t="s" s="0">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="G23" t="s" s="0">
         <v>15</v>

</xml_diff>